<commit_message>
Updated sheets to discussion status 20251008
</commit_message>
<xml_diff>
--- a/create_agent_directory/resources/abridged_enhanced_template.xlsx
+++ b/create_agent_directory/resources/abridged_enhanced_template.xlsx
@@ -298,22 +298,21 @@
     <comment ref="J1" authorId="0" shapeId="0">
       <text>
         <t>Scores Per Rubric
-This is a range between -10 and +10
+This is the score that is assigned to each rubric. It is a within the range of -10 and +10. Please note, this is NOT the score to assign to agent response, it is the score that each rubric carries.
 Format: Number</t>
       </text>
     </comment>
     <comment ref="K1" authorId="0" shapeId="0">
       <text>
         <t>Final Rubric Score
-If the score given is greater than 0, the final rubric score if Yes
-If the score given is lower than or equal to 0, the final rubric score is No
-OPTIONS: Yes, No
-Format: Dropdown</t>
+Score given to agent response for each rubric
+Format: Number</t>
       </text>
     </comment>
     <comment ref="L1" authorId="0" shapeId="0">
       <text>
         <t>Pass/Fail
+It is considered as Fail if the sum of scores from rubric is less than 80% of the highest possible score. (If the highest possible score is 40 and the agent response score was 35 then it is considered as a pass, but if it is 25 it is a fail)
 OPTIONS: Pass, Fail
 REQUIRED FIELD
 Format: Dropdown</t>
@@ -329,7 +328,13 @@
     </comment>
     <comment ref="N1" authorId="0" shapeId="0">
       <text>
-        <t>Success score (1-5)
+        <t>Quality score (1-5)
+Rate how well the agent solved the task given by the user (1: poor - 5: excellent) Example: Query: Schedule an appointment with Jane Doe on 10/8 at 10am and send email confirmation to her email
+Example for success rating 1 (poor): Agent did not schedule the appointment
+Example for success rating 2: Agent scheduled an appointment, but made a mistake with the invitee, date or time
+Example for success rating 3: Agent scheduled the appointment correctly, but did not confirm the appointment via email
+Example for success rating 4: Agent scheduled the appointment correctly, but omitted the invitee, date or time from the confirmation
+Example for success rating 5 (perfect): Agent scheduled the appointment and confirmed the invitee, date and time
 OPTIONS: 1, 2, 3, 4, 5
 REQUIRED FIELD
 Format: Number</t>
@@ -337,7 +342,8 @@
     </comment>
     <comment ref="O1" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">Justification for Success score
+        <t xml:space="preserve">Justification for Quality score
+Provide comments to justify/explain the quality score
 REQUIRED FIELD
 </t>
       </text>
@@ -1035,7 +1041,7 @@
         </is>
       </c>
     </row>
-    <row r="13" ht="71" customHeight="1">
+    <row r="13" ht="143" customHeight="1">
       <c r="A13" s="3" t="inlineStr">
         <is>
           <t>Scores Per Rubric</t>
@@ -1043,7 +1049,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>This is a range between -10 and +10</t>
+          <t>This is the score that is assigned to each rubric. It is a within the range of -10 and +10. Please note, this is NOT the score to assign to agent response, it is the score that each rubric carries.</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -1066,7 +1072,7 @@
         </is>
       </c>
     </row>
-    <row r="14" ht="125" customHeight="1">
+    <row r="14" ht="71" customHeight="1">
       <c r="A14" s="3" t="inlineStr">
         <is>
           <t>Final Rubric Score</t>
@@ -1074,20 +1080,15 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>If the score given is greater than 0, the final rubric score if Yes
-If the score given is lower than or equal to 0, the final rubric score is No</t>
+          <t>Score given to agent response for each rubric</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>Dropdown</t>
-        </is>
-      </c>
-      <c r="D14" s="3" t="inlineStr">
-        <is>
-          <t>Yes, No</t>
-        </is>
-      </c>
+          <t>Number</t>
+        </is>
+      </c>
+      <c r="D14" s="3" t="inlineStr"/>
       <c r="E14" s="3" t="inlineStr">
         <is>
           <t>Multiple</t>
@@ -1096,19 +1097,23 @@
       <c r="F14" s="3" t="inlineStr"/>
       <c r="G14" s="3" t="inlineStr">
         <is>
-          <t>Yes
-Yes 
-No</t>
-        </is>
-      </c>
-    </row>
-    <row r="15" ht="71" customHeight="1">
+          <t>8
+0
+-10</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="161" customHeight="1">
       <c r="A15" s="3" t="inlineStr">
         <is>
           <t>Pass/Fail</t>
         </is>
       </c>
-      <c r="B15" s="3" t="inlineStr"/>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>It is considered as Fail if the sum of scores from rubric is less than 80% of the highest possible score. (If the highest possible score is 40 and the agent response score was 35 then it is considered as a pass, but if it is 25 it is a fail)</t>
+        </is>
+      </c>
       <c r="C15" s="3" t="inlineStr">
         <is>
           <t>Dropdown</t>
@@ -1168,13 +1173,22 @@
         </is>
       </c>
     </row>
-    <row r="17" ht="71" customHeight="1">
+    <row r="17" ht="431" customHeight="1">
       <c r="A17" s="3" t="inlineStr">
         <is>
-          <t>Success score (1-5)</t>
-        </is>
-      </c>
-      <c r="B17" s="3" t="inlineStr"/>
+          <t>Quality score (1-5)</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Rate how well the agent solved the task given by the user (1: poor - 5: excellent) Example: Query: Schedule an appointment with Jane Doe on 10/8 at 10am and send email confirmation to her email
+Example for success rating 1 (poor): Agent did not schedule the appointment
+Example for success rating 2: Agent scheduled an appointment, but made a mistake with the invitee, date or time
+Example for success rating 3: Agent scheduled the appointment correctly, but did not confirm the appointment via email
+Example for success rating 4: Agent scheduled the appointment correctly, but omitted the invitee, date or time from the confirmation
+Example for success rating 5 (perfect): Agent scheduled the appointment and confirmed the invitee, date and time</t>
+        </is>
+      </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
           <t>Number</t>
@@ -1195,15 +1209,23 @@
           <t>Yes</t>
         </is>
       </c>
-      <c r="G17" s="3" t="inlineStr"/>
+      <c r="G17" s="3" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="18" ht="71" customHeight="1">
       <c r="A18" s="3" t="inlineStr">
         <is>
-          <t>Justification for Success score</t>
-        </is>
-      </c>
-      <c r="B18" s="3" t="inlineStr"/>
+          <t>Justification for Quality score</t>
+        </is>
+      </c>
+      <c r="B18" s="3" t="inlineStr">
+        <is>
+          <t>Provide comments to justify/explain the quality score</t>
+        </is>
+      </c>
       <c r="C18" s="3" t="inlineStr">
         <is>
           <t>Free text</t>
@@ -1328,12 +1350,12 @@
       </c>
       <c r="N1" s="6" t="inlineStr">
         <is>
-          <t>Success score (1-5)</t>
+          <t>Quality score (1-5)</t>
         </is>
       </c>
       <c r="O1" s="6" t="inlineStr">
         <is>
-          <t>Justification for Success score</t>
+          <t>Justification for Quality score</t>
         </is>
       </c>
     </row>
@@ -1366,8 +1388,8 @@
     <dataValidation sqref="J2:J1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
-      <formula1>"Yes,No"</formula1>
+    <dataValidation sqref="K2:K1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
     </dataValidation>
     <dataValidation sqref="L2:L1000" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="0" type="list">
       <formula1>"Pass,Fail"</formula1>

</xml_diff>